<commit_message>
Add API endpoints and infrastructure for activos management
Introduces new API endpoints for activos, activo_condicion, activo_estado, and activo_propiedad, supporting CRUD operations and CSV import/export. Adds supporting infrastructure files for database connections and autoloading. Updates .htaccess rules for improved routing and authorization header handling. Also includes new catalog, configuration, and manufacturing files, along with various supporting scripts and menu updates.
</commit_message>
<xml_diff>
--- a/public/manufactura/layout_importacion_ots.xlsx
+++ b/public/manufactura/layout_importacion_ots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp_new\htdocs\assistpro_kardex_fc\public\manufactura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1279441A-5717-4D99-82E7-99852763064A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F747E4AA-06D5-4991-BEC4-E00ED75D5396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="45">
   <si>
     <t>OT_Cliente</t>
   </si>
@@ -56,9 +54,6 @@
     <t>Fecha Compromiso</t>
   </si>
   <si>
-    <t>LP</t>
-  </si>
-  <si>
     <t>A6-43019-001B2-110</t>
   </si>
   <si>
@@ -153,6 +148,27 @@
   </si>
   <si>
     <t>45906094</t>
+  </si>
+  <si>
+    <t>BL_ORIGEN</t>
+  </si>
+  <si>
+    <t>BL_DESTINO</t>
+  </si>
+  <si>
+    <t>LP_CONTENEDOR</t>
+  </si>
+  <si>
+    <t>LP_PALLET</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>LP20252512-00001</t>
+  </si>
+  <si>
+    <t>LP20252512-00002</t>
   </si>
 </sst>
 </file>
@@ -585,10 +601,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -599,11 +615,13 @@
     <col min="4" max="4" width="10.109375" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.44140625" style="5"/>
+    <col min="7" max="7" width="11.44140625" style="5"/>
+    <col min="8" max="8" width="35.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.109375" style="5" customWidth="1"/>
+    <col min="10" max="16384" width="11.44140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -622,16 +640,25 @@
       <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" s="5">
         <v>12</v>
@@ -639,17 +666,20 @@
       <c r="F2" s="3">
         <v>45940</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <f>+A2+1</f>
         <v>45906095</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" s="5">
         <v>12</v>
@@ -657,17 +687,20 @@
       <c r="F3" s="3">
         <v>45940</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <f t="shared" ref="A4:A23" si="0">+A3+1</f>
         <v>45906096</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="5">
         <v>12</v>
@@ -675,182 +708,212 @@
       <c r="F4" s="3">
         <v>45940</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <f t="shared" si="0"/>
+        <v>45906097</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="5">
+        <v>12</v>
+      </c>
+      <c r="F5" s="3">
+        <v>45940</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
-        <f t="shared" si="0"/>
-        <v>45906097</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="5">
-        <v>12</v>
-      </c>
-      <c r="F5" s="3">
-        <v>45940</v>
-      </c>
-      <c r="G5" s="5" t="s">
+      <c r="I5" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <f t="shared" si="0"/>
+        <v>45906098</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="5">
+        <v>12</v>
+      </c>
+      <c r="F6" s="3">
+        <v>45940</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
-        <f t="shared" si="0"/>
-        <v>45906098</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="5">
-        <v>12</v>
-      </c>
-      <c r="F6" s="3">
-        <v>45940</v>
-      </c>
-      <c r="G6" s="5" t="s">
+      <c r="I6" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <f t="shared" si="0"/>
+        <v>45906099</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="5">
+        <v>12</v>
+      </c>
+      <c r="F7" s="3">
+        <v>45940</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
-        <f t="shared" si="0"/>
-        <v>45906099</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="5">
-        <v>12</v>
-      </c>
-      <c r="F7" s="3">
-        <v>45940</v>
-      </c>
-      <c r="G7" s="5" t="s">
+      <c r="I7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
+        <f t="shared" si="0"/>
+        <v>45906100</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="5">
+        <v>12</v>
+      </c>
+      <c r="F8" s="3">
+        <v>45940</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I8" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <f t="shared" si="0"/>
+        <v>45906101</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="5">
+        <v>12</v>
+      </c>
+      <c r="F9" s="3">
+        <v>45940</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <f t="shared" si="0"/>
+        <v>45906102</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="5">
+        <v>12</v>
+      </c>
+      <c r="F10" s="3">
+        <v>45940</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <f t="shared" si="0"/>
+        <v>45906103</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="5">
+        <v>12</v>
+      </c>
+      <c r="F11" s="3">
+        <v>45940</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
+        <f t="shared" si="0"/>
+        <v>45906104</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="5">
+        <v>12</v>
+      </c>
+      <c r="F12" s="3">
+        <v>45940</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
+        <f t="shared" si="0"/>
+        <v>45906105</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="5">
+        <v>12</v>
+      </c>
+      <c r="F13" s="3">
+        <v>45940</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
+        <f t="shared" si="0"/>
+        <v>45906106</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
-        <f t="shared" si="0"/>
-        <v>45906100</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="5">
-        <v>12</v>
-      </c>
-      <c r="F8" s="3">
-        <v>45940</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
-        <f t="shared" si="0"/>
-        <v>45906101</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="5">
-        <v>12</v>
-      </c>
-      <c r="F9" s="3">
-        <v>45940</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
-        <f t="shared" si="0"/>
-        <v>45906102</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="5">
-        <v>12</v>
-      </c>
-      <c r="F10" s="3">
-        <v>45940</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
-        <f t="shared" si="0"/>
-        <v>45906103</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="5">
-        <v>12</v>
-      </c>
-      <c r="F11" s="3">
-        <v>45940</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
-        <f t="shared" si="0"/>
-        <v>45906104</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="5">
-        <v>12</v>
-      </c>
-      <c r="F12" s="3">
-        <v>45940</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
-        <f t="shared" si="0"/>
-        <v>45906105</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="5">
-        <v>12</v>
-      </c>
-      <c r="F13" s="3">
-        <v>45940</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
-        <f t="shared" si="0"/>
-        <v>45906106</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>11</v>
       </c>
       <c r="E14" s="5">
         <v>24</v>
@@ -858,35 +921,41 @@
       <c r="F14" s="3">
         <v>45940</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="H14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
+        <f t="shared" si="0"/>
+        <v>45906107</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="5">
+        <v>12</v>
+      </c>
+      <c r="F15" s="3">
+        <v>45940</v>
+      </c>
+      <c r="H15" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
-        <f t="shared" si="0"/>
-        <v>45906107</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="5">
-        <v>12</v>
-      </c>
-      <c r="F15" s="3">
-        <v>45940</v>
-      </c>
-      <c r="G15" s="5" t="s">
+      <c r="I15" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
+        <f t="shared" si="0"/>
+        <v>45906108</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="5">
-        <f t="shared" si="0"/>
-        <v>45906108</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="E16" s="5">
         <v>24</v>
@@ -894,17 +963,20 @@
       <c r="F16" s="3">
         <v>45940</v>
       </c>
-      <c r="G16" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <f t="shared" si="0"/>
         <v>45906109</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E17" s="5">
         <v>24</v>
@@ -912,17 +984,20 @@
       <c r="F17" s="3">
         <v>45940</v>
       </c>
-      <c r="G17" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <f t="shared" si="0"/>
         <v>45906110</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E18" s="5">
         <v>24</v>
@@ -930,71 +1005,83 @@
       <c r="F18" s="3">
         <v>45940</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="H18" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="5">
+        <f t="shared" si="0"/>
+        <v>45906111</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="5">
+        <v>12</v>
+      </c>
+      <c r="F19" s="3">
+        <v>45940</v>
+      </c>
+      <c r="H19" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="5">
-        <f t="shared" si="0"/>
-        <v>45906111</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="5">
-        <v>12</v>
-      </c>
-      <c r="F19" s="3">
-        <v>45940</v>
-      </c>
-      <c r="G19" s="5" t="s">
+      <c r="I19" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="5">
+        <f t="shared" si="0"/>
+        <v>45906112</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="5">
+        <v>12</v>
+      </c>
+      <c r="F20" s="3">
+        <v>45940</v>
+      </c>
+      <c r="H20" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="5">
-        <f t="shared" si="0"/>
-        <v>45906112</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="5">
-        <v>12</v>
-      </c>
-      <c r="F20" s="3">
-        <v>45940</v>
-      </c>
-      <c r="G20" s="5" t="s">
+      <c r="I20" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
+        <f t="shared" si="0"/>
+        <v>45906113</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="5">
+        <v>12</v>
+      </c>
+      <c r="F21" s="3">
+        <v>45940</v>
+      </c>
+      <c r="H21" s="5" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="5">
-        <f t="shared" si="0"/>
-        <v>45906113</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="5">
-        <v>12</v>
-      </c>
-      <c r="F21" s="3">
-        <v>45940</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I21" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <f t="shared" si="0"/>
         <v>45906114</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E22" s="5">
         <v>24</v>
@@ -1002,17 +1089,20 @@
       <c r="F22" s="3">
         <v>45940</v>
       </c>
-      <c r="G22" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H22" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <f t="shared" si="0"/>
         <v>45906115</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E23" s="5">
         <v>24</v>
@@ -1020,32 +1110,35 @@
       <c r="F23" s="3">
         <v>45940</v>
       </c>
-      <c r="G23" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H23" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
     </row>
   </sheetData>
@@ -1060,7 +1153,7 @@
       <formula>"error"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7">
+  <conditionalFormatting sqref="J7">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
       <formula>"error"</formula>
     </cfRule>
@@ -1080,14 +1173,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="64193f95-c656-451f-9a5b-99be98c50541" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100DF48C11443F2214D9C72AD5B1E401277" ma:contentTypeVersion="9" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="a14549906a4bf477b142a5f1c02b308a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="64193f95-c656-451f-9a5b-99be98c50541" xmlns:ns4="65450c67-5873-4663-8486-ed0d7a198d81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="11a6802feaebdd2610c16ec093506f24" ns3:_="" ns4:_="">
     <xsd:import namespace="64193f95-c656-451f-9a5b-99be98c50541"/>
@@ -1282,6 +1367,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="64193f95-c656-451f-9a5b-99be98c50541" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A556156-26F2-452C-BB64-908F60A0019B}">
   <ds:schemaRefs>
@@ -1291,23 +1384,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97878285-DD27-4FB4-B16C-B2AEACAFDB4D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="64193f95-c656-451f-9a5b-99be98c50541"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="65450c67-5873-4663-8486-ed0d7a198d81"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26FDEA69-EA0B-4E9E-8AA8-F7A0BBF6BD7B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1324,4 +1400,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97878285-DD27-4FB4-B16C-B2AEACAFDB4D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="64193f95-c656-451f-9a5b-99be98c50541"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="65450c67-5873-4663-8486-ed0d7a198d81"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>